<commit_message>
now checks if entry already exists by BRnum in excel file - if it does, skip it + alot of refactoring - preprared for KISS/DRY tomorrow
</commit_message>
<xml_diff>
--- a/src/main/java/org/example/util/data/GRI_2017_2020_TEST.xlsx
+++ b/src/main/java/org/example/util/data/GRI_2017_2020_TEST.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Specialisterne - Opgaver\Uge 4\PDF_DOWNLOADER\src\main\java\org\example\util\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rober\OneDrive\Coding\GitHub Desktop Projects\PDF_DOWNLOADER\src\main\java\org\example\util\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC4A5802-651F-4FE9-B84A-800C5921A08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE7ACDA-6425-4A54-8ED4-B809E51A4A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5160" yWindow="1890" windowWidth="41280" windowHeight="17115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="19" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="148">
   <si>
     <t>BRnum</t>
   </si>
@@ -176,12 +176,6 @@
     <t>Europe</t>
   </si>
   <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>Non - GRI</t>
   </si>
   <si>
@@ -200,9 +194,6 @@
     <t>Telecommunications</t>
   </si>
   <si>
-    <t>27-11-2017</t>
-  </si>
-  <si>
     <t>Umwelterklärung 2016/2017</t>
   </si>
   <si>
@@ -212,6 +203,30 @@
     <t>http://database.globalreporting.org/reports/320a3f6f-83d3-e711-811e-e0071b6641b1</t>
   </si>
   <si>
+    <t>BR50041</t>
+  </si>
+  <si>
+    <t>A.R.Peissig-Dolder</t>
+  </si>
+  <si>
+    <t>SME</t>
+  </si>
+  <si>
+    <t>Non-listed</t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
+  <si>
+    <t>Erster Bericht zur Nachhaltigkeit</t>
+  </si>
+  <si>
+    <t>http://arpeissig.at/wp-content/uploads/2016/02/D7_NHB_ARP_Final_2.pdf</t>
+  </si>
+  <si>
+    <t>http://database.globalreporting.org/reports/bfe8fd47-dc6c-ea11-a811-000d3ab11761</t>
+  </si>
+  <si>
     <t>BR50043</t>
   </si>
   <si>
@@ -224,9 +239,6 @@
     <t>Italy</t>
   </si>
   <si>
-    <t>26-5-2017</t>
-  </si>
-  <si>
     <t>Integrated Report 2016</t>
   </si>
   <si>
@@ -263,33 +275,6 @@
     <t>http://database.globalreporting.org/reports/0b24f5a3-4e36-e711-80ea-3863bb354df0</t>
   </si>
   <si>
-    <t>BR50041</t>
-  </si>
-  <si>
-    <t>A.R.Peissig-Dolder</t>
-  </si>
-  <si>
-    <t>SME</t>
-  </si>
-  <si>
-    <t>Non-listed</t>
-  </si>
-  <si>
-    <t>Chemicals</t>
-  </si>
-  <si>
-    <t>22-3-2020</t>
-  </si>
-  <si>
-    <t>Erster Bericht zur Nachhaltigkeit</t>
-  </si>
-  <si>
-    <t>http://arpeissig.at/wp-content/uploads/2016/02/D7_NHB_ARP_Final_2.pdf</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/bfe8fd47-dc6c-ea11-a811-000d3ab11761</t>
-  </si>
-  <si>
     <t>BR50044</t>
   </si>
   <si>
@@ -305,9 +290,6 @@
     <t>United Kingdom of Great Britain and Northern Ireland</t>
   </si>
   <si>
-    <t>2-1-2018</t>
-  </si>
-  <si>
     <t>AA plc Annual Report and Accounts 2017</t>
   </si>
   <si>
@@ -335,9 +317,6 @@
     <t>Asia</t>
   </si>
   <si>
-    <t>7-8-2017</t>
-  </si>
-  <si>
     <t>2016 Sustainability Report</t>
   </si>
   <si>
@@ -362,9 +341,6 @@
     <t>Taiwan</t>
   </si>
   <si>
-    <t>26-5-2020</t>
-  </si>
-  <si>
     <t>2016 Corporate Social Responsibility Report</t>
   </si>
   <si>
@@ -386,9 +362,6 @@
     <t>Sweden</t>
   </si>
   <si>
-    <t>13-2-2018</t>
-  </si>
-  <si>
     <t>Sustainability Report 2016/2017</t>
   </si>
   <si>
@@ -416,9 +389,6 @@
     <t>Finland</t>
   </si>
   <si>
-    <t>4-9-2017</t>
-  </si>
-  <si>
     <t>Sustainable Campus Charter Report of Aalto University 2016</t>
   </si>
   <si>
@@ -443,9 +413,6 @@
     <t>Switzerland</t>
   </si>
   <si>
-    <t>26-3-2020</t>
-  </si>
-  <si>
     <t>Nachhaltige Entwicklung im Kanton Aargau 2016</t>
   </si>
   <si>
@@ -464,9 +431,6 @@
     <t>Financial Services</t>
   </si>
   <si>
-    <t>1-6-2018</t>
-  </si>
-  <si>
     <t>AKB Nachhaltigkeitsbericht 2016</t>
   </si>
   <si>
@@ -491,9 +455,6 @@
     <t>Lithuania</t>
   </si>
   <si>
-    <t>15-1-2018</t>
-  </si>
-  <si>
     <t>2016 Social Responsibility Progress Report</t>
   </si>
   <si>
@@ -513,9 +474,6 @@
   </si>
   <si>
     <t>France</t>
-  </si>
-  <si>
-    <t>27-7-2017</t>
   </si>
   <si>
     <t>Document de Référence 2016</t>
@@ -585,8 +543,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{97F51F2D-A06D-473C-938C-9A83B79C5A71}"/>
@@ -908,7 +867,7 @@
   <dimension ref="A1:AO13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D13" sqref="A1:AO13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,28 +1042,28 @@
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
         <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="I2" t="s">
         <v>43</v>
@@ -1115,48 +1074,24 @@
       <c r="K2" t="s">
         <v>44</v>
       </c>
-      <c r="L2" t="s">
-        <v>79</v>
+      <c r="L2" s="1">
+        <v>43912</v>
       </c>
       <c r="M2" t="s">
-        <v>80</v>
-      </c>
-      <c r="N2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2">
+        <v>2017</v>
+      </c>
+      <c r="P2" t="s">
         <v>45</v>
       </c>
-      <c r="O2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>46</v>
-      </c>
-      <c r="R2" t="s">
-        <v>46</v>
-      </c>
-      <c r="S2" t="s">
-        <v>46</v>
-      </c>
       <c r="T2" t="s">
         <v>41</v>
       </c>
-      <c r="U2" t="s">
-        <v>46</v>
-      </c>
-      <c r="V2" t="s">
-        <v>46</v>
-      </c>
       <c r="W2" t="s">
         <v>41</v>
       </c>
-      <c r="X2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>46</v>
-      </c>
       <c r="Z2" t="s">
         <v>41</v>
       </c>
@@ -1169,67 +1104,37 @@
       <c r="AC2" t="s">
         <v>41</v>
       </c>
-      <c r="AD2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>46</v>
-      </c>
       <c r="AL2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="AO2" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>50</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s">
         <v>43</v>
@@ -1240,124 +1145,70 @@
       <c r="K3" t="s">
         <v>44</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1">
+        <v>43066</v>
+      </c>
+      <c r="M3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3">
+        <v>2017</v>
+      </c>
+      <c r="P3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T3" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO3" t="s">
         <v>53</v>
-      </c>
-      <c r="M3" t="s">
-        <v>54</v>
-      </c>
-      <c r="N3" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3" t="s">
-        <v>46</v>
-      </c>
-      <c r="S3" t="s">
-        <v>46</v>
-      </c>
-      <c r="T3" t="s">
-        <v>41</v>
-      </c>
-      <c r="U3" t="s">
-        <v>46</v>
-      </c>
-      <c r="V3" t="s">
-        <v>46</v>
-      </c>
-      <c r="W3" t="s">
-        <v>41</v>
-      </c>
-      <c r="X3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
         <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
         <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="I4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="J4" t="s">
         <v>30</v>
@@ -1365,54 +1216,48 @@
       <c r="K4" t="s">
         <v>44</v>
       </c>
-      <c r="L4" t="s">
-        <v>61</v>
+      <c r="L4" s="1">
+        <v>42881</v>
       </c>
       <c r="M4" t="s">
-        <v>62</v>
-      </c>
-      <c r="N4" t="s">
-        <v>45</v>
+        <v>66</v>
+      </c>
+      <c r="N4">
+        <v>2017</v>
       </c>
       <c r="O4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="P4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="Q4" t="s">
-        <v>65</v>
-      </c>
-      <c r="R4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S4" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="T4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="U4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="V4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W4" t="s">
+        <v>41</v>
+      </c>
+      <c r="X4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA4" t="s">
         <v>67</v>
       </c>
-      <c r="W4" t="s">
-        <v>41</v>
-      </c>
-      <c r="X4" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>63</v>
-      </c>
       <c r="AB4" t="s">
         <v>41</v>
       </c>
@@ -1420,16 +1265,16 @@
         <v>41</v>
       </c>
       <c r="AD4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AE4" t="s">
         <v>41</v>
       </c>
       <c r="AF4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AG4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AH4" t="s">
         <v>41</v>
@@ -1438,51 +1283,45 @@
         <v>41</v>
       </c>
       <c r="AJ4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="AL4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="AM4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="AO4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
         <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="I5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="J5" t="s">
         <v>30</v>
@@ -1490,48 +1329,24 @@
       <c r="K5" t="s">
         <v>44</v>
       </c>
-      <c r="L5" t="s">
-        <v>88</v>
+      <c r="L5" s="1">
+        <v>43102</v>
       </c>
       <c r="M5" t="s">
-        <v>89</v>
-      </c>
-      <c r="N5" t="s">
+        <v>83</v>
+      </c>
+      <c r="N5">
+        <v>2017</v>
+      </c>
+      <c r="P5" t="s">
         <v>45</v>
       </c>
-      <c r="O5" t="s">
-        <v>46</v>
-      </c>
-      <c r="P5" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>46</v>
-      </c>
-      <c r="R5" t="s">
-        <v>46</v>
-      </c>
-      <c r="S5" t="s">
-        <v>46</v>
-      </c>
       <c r="T5" t="s">
         <v>41</v>
       </c>
-      <c r="U5" t="s">
-        <v>46</v>
-      </c>
-      <c r="V5" t="s">
-        <v>46</v>
-      </c>
       <c r="W5" t="s">
         <v>41</v>
       </c>
-      <c r="X5" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>46</v>
-      </c>
       <c r="Z5" t="s">
         <v>41</v>
       </c>
@@ -1544,244 +1359,166 @@
       <c r="AC5" t="s">
         <v>41</v>
       </c>
-      <c r="AD5" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>46</v>
-      </c>
       <c r="AL5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="AO5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
         <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
         <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" t="s">
+        <v>90</v>
+      </c>
+      <c r="K6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="1">
+        <v>42954</v>
+      </c>
+      <c r="M6" t="s">
+        <v>92</v>
+      </c>
+      <c r="N6">
+        <v>2017</v>
+      </c>
+      <c r="O6" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>69</v>
+      </c>
+      <c r="T6" t="s">
+        <v>41</v>
+      </c>
+      <c r="W6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL6" t="s">
         <v>94</v>
       </c>
-      <c r="I6" t="s">
+      <c r="AO6" t="s">
         <v>95</v>
-      </c>
-      <c r="J6" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6" t="s">
-        <v>97</v>
-      </c>
-      <c r="L6" t="s">
-        <v>98</v>
-      </c>
-      <c r="M6" t="s">
-        <v>99</v>
-      </c>
-      <c r="N6" t="s">
-        <v>45</v>
-      </c>
-      <c r="O6" t="s">
-        <v>41</v>
-      </c>
-      <c r="P6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>65</v>
-      </c>
-      <c r="R6" t="s">
-        <v>46</v>
-      </c>
-      <c r="S6" t="s">
-        <v>46</v>
-      </c>
-      <c r="T6" t="s">
-        <v>41</v>
-      </c>
-      <c r="U6" t="s">
-        <v>46</v>
-      </c>
-      <c r="V6" t="s">
-        <v>46</v>
-      </c>
-      <c r="W6" t="s">
-        <v>41</v>
-      </c>
-      <c r="X6" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>100</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>101</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>46</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
         <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="I7" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="J7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="K7" t="s">
-        <v>97</v>
-      </c>
-      <c r="L7" t="s">
-        <v>107</v>
+        <v>91</v>
+      </c>
+      <c r="L7" s="1">
+        <v>43977</v>
       </c>
       <c r="M7" t="s">
-        <v>108</v>
-      </c>
-      <c r="N7" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" t="s">
-        <v>46</v>
+        <v>100</v>
+      </c>
+      <c r="N7">
+        <v>2017</v>
       </c>
       <c r="P7" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="Q7" t="s">
-        <v>109</v>
-      </c>
-      <c r="R7" t="s">
-        <v>46</v>
-      </c>
-      <c r="S7" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="T7" t="s">
         <v>41</v>
       </c>
-      <c r="U7" t="s">
-        <v>46</v>
-      </c>
-      <c r="V7" t="s">
-        <v>46</v>
-      </c>
       <c r="W7" t="s">
         <v>41</v>
       </c>
-      <c r="X7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>46</v>
-      </c>
       <c r="Z7" t="s">
         <v>41</v>
       </c>
@@ -1794,70 +1531,37 @@
       <c r="AC7" t="s">
         <v>41</v>
       </c>
-      <c r="AD7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>46</v>
-      </c>
       <c r="AO7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
         <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
         <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H8" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="I8" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="J8" t="s">
         <v>30</v>
@@ -1865,124 +1569,97 @@
       <c r="K8" t="s">
         <v>44</v>
       </c>
-      <c r="L8" t="s">
-        <v>115</v>
+      <c r="L8" s="1">
+        <v>43144</v>
       </c>
       <c r="M8" t="s">
-        <v>116</v>
-      </c>
-      <c r="N8" t="s">
-        <v>45</v>
+        <v>107</v>
+      </c>
+      <c r="N8">
+        <v>2017</v>
       </c>
       <c r="O8" t="s">
         <v>41</v>
       </c>
       <c r="P8" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="Q8" t="s">
+        <v>101</v>
+      </c>
+      <c r="T8" t="s">
+        <v>41</v>
+      </c>
+      <c r="W8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL8" t="s">
         <v>109</v>
       </c>
-      <c r="R8" t="s">
-        <v>46</v>
-      </c>
-      <c r="S8" t="s">
-        <v>46</v>
-      </c>
-      <c r="T8" t="s">
-        <v>41</v>
-      </c>
-      <c r="U8" t="s">
-        <v>46</v>
-      </c>
-      <c r="V8" t="s">
-        <v>46</v>
-      </c>
-      <c r="W8" t="s">
-        <v>41</v>
-      </c>
-      <c r="X8" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>117</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>118</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>46</v>
-      </c>
       <c r="AO8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D9" t="s">
         <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="G9" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="I9" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J9" t="s">
         <v>30</v>
@@ -1990,48 +1667,24 @@
       <c r="K9" t="s">
         <v>44</v>
       </c>
-      <c r="L9" t="s">
-        <v>125</v>
+      <c r="L9" s="1">
+        <v>42982</v>
       </c>
       <c r="M9" t="s">
-        <v>126</v>
-      </c>
-      <c r="N9" t="s">
+        <v>116</v>
+      </c>
+      <c r="N9">
+        <v>2017</v>
+      </c>
+      <c r="P9" t="s">
         <v>45</v>
       </c>
-      <c r="O9" t="s">
-        <v>46</v>
-      </c>
-      <c r="P9" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>46</v>
-      </c>
-      <c r="R9" t="s">
-        <v>46</v>
-      </c>
-      <c r="S9" t="s">
-        <v>46</v>
-      </c>
       <c r="T9" t="s">
         <v>41</v>
       </c>
-      <c r="U9" t="s">
-        <v>46</v>
-      </c>
-      <c r="V9" t="s">
-        <v>46</v>
-      </c>
       <c r="W9" t="s">
         <v>41</v>
       </c>
-      <c r="X9" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>46</v>
-      </c>
       <c r="Z9" t="s">
         <v>41</v>
       </c>
@@ -2044,70 +1697,43 @@
       <c r="AC9" t="s">
         <v>41</v>
       </c>
-      <c r="AD9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>46</v>
-      </c>
       <c r="AL9" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="AM9" t="s">
-        <v>128</v>
-      </c>
-      <c r="AN9" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="AO9" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
         <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" t="s">
         <v>122</v>
       </c>
-      <c r="G10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" t="s">
-        <v>132</v>
-      </c>
       <c r="I10" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="J10" t="s">
         <v>30</v>
@@ -2115,48 +1741,24 @@
       <c r="K10" t="s">
         <v>44</v>
       </c>
-      <c r="L10" t="s">
-        <v>134</v>
+      <c r="L10" s="1">
+        <v>43916</v>
       </c>
       <c r="M10" t="s">
-        <v>135</v>
-      </c>
-      <c r="N10" t="s">
+        <v>124</v>
+      </c>
+      <c r="N10">
+        <v>2017</v>
+      </c>
+      <c r="P10" t="s">
         <v>45</v>
       </c>
-      <c r="O10" t="s">
-        <v>46</v>
-      </c>
-      <c r="P10" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>46</v>
-      </c>
-      <c r="R10" t="s">
-        <v>46</v>
-      </c>
-      <c r="S10" t="s">
-        <v>46</v>
-      </c>
       <c r="T10" t="s">
         <v>41</v>
       </c>
-      <c r="U10" t="s">
-        <v>46</v>
-      </c>
-      <c r="V10" t="s">
-        <v>46</v>
-      </c>
       <c r="W10" t="s">
         <v>41</v>
       </c>
-      <c r="X10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>46</v>
-      </c>
       <c r="Z10" t="s">
         <v>41</v>
       </c>
@@ -2169,70 +1771,40 @@
       <c r="AC10" t="s">
         <v>41</v>
       </c>
-      <c r="AD10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK10" t="s">
-        <v>46</v>
-      </c>
       <c r="AL10" t="s">
-        <v>136</v>
-      </c>
-      <c r="AM10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN10" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="AO10" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="D11" t="s">
         <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
         <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H11" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="I11" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="J11" t="s">
         <v>30</v>
@@ -2240,48 +1812,30 @@
       <c r="K11" t="s">
         <v>44</v>
       </c>
-      <c r="L11" t="s">
-        <v>141</v>
+      <c r="L11" s="1">
+        <v>43252</v>
       </c>
       <c r="M11" t="s">
-        <v>142</v>
-      </c>
-      <c r="N11" t="s">
-        <v>45</v>
+        <v>130</v>
+      </c>
+      <c r="N11">
+        <v>2017</v>
       </c>
       <c r="O11" t="s">
         <v>41</v>
       </c>
       <c r="P11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="Q11" t="s">
-        <v>65</v>
-      </c>
-      <c r="R11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S11" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="T11" t="s">
         <v>41</v>
       </c>
-      <c r="U11" t="s">
-        <v>46</v>
-      </c>
-      <c r="V11" t="s">
-        <v>46</v>
-      </c>
       <c r="W11" t="s">
         <v>41</v>
       </c>
-      <c r="X11" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>46</v>
-      </c>
       <c r="Z11" t="s">
         <v>41</v>
       </c>
@@ -2295,7 +1849,7 @@
         <v>41</v>
       </c>
       <c r="AD11" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="AE11" t="s">
         <v>41</v>
@@ -2315,49 +1869,43 @@
       <c r="AJ11" t="s">
         <v>41</v>
       </c>
-      <c r="AK11" t="s">
-        <v>46</v>
-      </c>
       <c r="AL11" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="AM11" t="s">
-        <v>145</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>46</v>
+        <v>133</v>
       </c>
       <c r="AO11" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
         <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D12" t="s">
         <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F12" t="s">
         <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H12" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="I12" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="J12" t="s">
         <v>30</v>
@@ -2365,48 +1913,24 @@
       <c r="K12" t="s">
         <v>44</v>
       </c>
-      <c r="L12" t="s">
-        <v>150</v>
+      <c r="L12" s="1">
+        <v>43115</v>
       </c>
       <c r="M12" t="s">
-        <v>151</v>
-      </c>
-      <c r="N12" t="s">
+        <v>138</v>
+      </c>
+      <c r="N12">
+        <v>2017</v>
+      </c>
+      <c r="P12" t="s">
         <v>45</v>
       </c>
-      <c r="O12" t="s">
-        <v>46</v>
-      </c>
-      <c r="P12" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>46</v>
-      </c>
-      <c r="R12" t="s">
-        <v>46</v>
-      </c>
-      <c r="S12" t="s">
-        <v>46</v>
-      </c>
       <c r="T12" t="s">
         <v>41</v>
       </c>
-      <c r="U12" t="s">
-        <v>46</v>
-      </c>
-      <c r="V12" t="s">
-        <v>46</v>
-      </c>
       <c r="W12" t="s">
         <v>41</v>
       </c>
-      <c r="X12" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>46</v>
-      </c>
       <c r="Z12" t="s">
         <v>41</v>
       </c>
@@ -2419,70 +1943,40 @@
       <c r="AC12" t="s">
         <v>41</v>
       </c>
-      <c r="AD12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK12" t="s">
-        <v>46</v>
-      </c>
       <c r="AL12" t="s">
-        <v>152</v>
-      </c>
-      <c r="AM12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN12" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="AO12" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="B13" t="s">
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D13" t="s">
         <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
         <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H13" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="I13" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="J13" t="s">
         <v>30</v>
@@ -2490,48 +1984,24 @@
       <c r="K13" t="s">
         <v>44</v>
       </c>
-      <c r="L13" t="s">
-        <v>158</v>
+      <c r="L13" s="1">
+        <v>42943</v>
       </c>
       <c r="M13" t="s">
-        <v>159</v>
-      </c>
-      <c r="N13" t="s">
+        <v>145</v>
+      </c>
+      <c r="N13">
+        <v>2017</v>
+      </c>
+      <c r="P13" t="s">
         <v>45</v>
       </c>
-      <c r="O13" t="s">
-        <v>46</v>
-      </c>
-      <c r="P13" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>46</v>
-      </c>
-      <c r="R13" t="s">
-        <v>46</v>
-      </c>
-      <c r="S13" t="s">
-        <v>46</v>
-      </c>
       <c r="T13" t="s">
         <v>41</v>
       </c>
-      <c r="U13" t="s">
-        <v>46</v>
-      </c>
-      <c r="V13" t="s">
-        <v>46</v>
-      </c>
       <c r="W13" t="s">
         <v>41</v>
       </c>
-      <c r="X13" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>46</v>
-      </c>
       <c r="Z13" t="s">
         <v>41</v>
       </c>
@@ -2544,41 +2014,11 @@
       <c r="AC13" t="s">
         <v>41</v>
       </c>
-      <c r="AD13" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI13" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK13" t="s">
-        <v>46</v>
-      </c>
       <c r="AL13" t="s">
-        <v>160</v>
-      </c>
-      <c r="AM13" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>46</v>
+        <v>146</v>
       </c>
       <c r="AO13" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2597,12 +2037,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BD87EC79D7AB454591EAFECBD90626D9" ma:contentTypeVersion="3" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="0d3d7e2407b21afa2d30d9f4658ecfdd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a15b57ec-90af-49ba-a0a2-d3f0af0f9931" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a24a46ed92df228c743fe265ed7e3ec" ns2:_="">
     <xsd:import namespace="a15b57ec-90af-49ba-a0a2-d3f0af0f9931"/>
@@ -2740,6 +2174,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F88078F6-43DB-49DB-9553-D1E65F1B4C15}">
   <ds:schemaRefs>
@@ -2749,15 +2189,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D55DEAC-2583-419A-AEEA-EE94A1A19F78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5D91F3F-1996-4144-8D6F-BAF2247286FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2773,4 +2204,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D55DEAC-2583-419A-AEEA-EE94A1A19F78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add SOLID, DRY, KISS + refactoring + logging + timeout on download
</commit_message>
<xml_diff>
--- a/src/main/java/org/example/util/data/GRI_2017_2020_TEST.xlsx
+++ b/src/main/java/org/example/util/data/GRI_2017_2020_TEST.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rober\OneDrive\Coding\GitHub Desktop Projects\PDF_DOWNLOADER\src\main\java\org\example\util\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/35d016b557654f51/Coding/GitHub Desktop Projects/PDF_DOWNLOADER/src/main/java/org/example/util/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE7ACDA-6425-4A54-8ED4-B809E51A4A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="6_{E80B89F1-FD20-43B6-9A20-747F04E0BE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E24A5591-F137-41AE-8F30-CC1E03CD11E9}"/>
   <bookViews>
     <workbookView xWindow="5160" yWindow="1890" windowWidth="41280" windowHeight="17115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="127">
   <si>
     <t>BRnum</t>
   </si>
@@ -420,69 +420,6 @@
   </si>
   <si>
     <t>http://database.globalreporting.org/reports/5a1f9f2b-fe6f-ea11-a811-000d3ab11761</t>
-  </si>
-  <si>
-    <t>BR50050</t>
-  </si>
-  <si>
-    <t>Aargauische Kantonalbank</t>
-  </si>
-  <si>
-    <t>Financial Services</t>
-  </si>
-  <si>
-    <t>AKB Nachhaltigkeitsbericht 2016</t>
-  </si>
-  <si>
-    <t>Not Used</t>
-  </si>
-  <si>
-    <t>https://www.akb.ch/documents/30573/92310/nachhaltigkeitsbericht-2016.pdf</t>
-  </si>
-  <si>
-    <t>https://www.akb.ch/die-akb/kommunikation-medien/geschaeftsberichte</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/c3c6ed85-2a63-e811-8136-e0071b6641b1</t>
-  </si>
-  <si>
-    <t>BR50051</t>
-  </si>
-  <si>
-    <t>AB Klaipėdos Nafta</t>
-  </si>
-  <si>
-    <t>Lithuania</t>
-  </si>
-  <si>
-    <t>2016 Social Responsibility Progress Report</t>
-  </si>
-  <si>
-    <t>http://www.eugesta.lt/assets/SOCIALINES-ATSAKOMYBES-ATASKAITA-2016.pdf</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/92a17eed-e2f9-e711-8141-e0071b647f61</t>
-  </si>
-  <si>
-    <t>BR50052</t>
-  </si>
-  <si>
-    <t>AB science</t>
-  </si>
-  <si>
-    <t>Healthcare Products</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Document de Référence 2016</t>
-  </si>
-  <si>
-    <t>http://www.ab-science.com/file_bdd/content/1480493978_DDRVF.pdf</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/76787066-df71-e711-812b-e0071b647f61</t>
   </si>
 </sst>
 </file>
@@ -565,6 +502,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -864,55 +805,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:AO13"/>
+  <dimension ref="A1:AO52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="A1:AO13"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="31" customWidth="1"/>
-    <col min="9" max="9" width="48.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" customWidth="1"/>
-    <col min="11" max="11" width="28.28515625" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="113.28515625" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" customWidth="1"/>
-    <col min="17" max="17" width="29" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" customWidth="1"/>
-    <col min="19" max="19" width="68.140625" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" customWidth="1"/>
-    <col min="21" max="21" width="30.42578125" customWidth="1"/>
-    <col min="22" max="22" width="23.42578125" customWidth="1"/>
-    <col min="23" max="23" width="34.85546875" customWidth="1"/>
-    <col min="24" max="24" width="24.7109375" customWidth="1"/>
-    <col min="25" max="25" width="20.28515625" customWidth="1"/>
-    <col min="26" max="26" width="32.28515625" customWidth="1"/>
-    <col min="27" max="27" width="32" customWidth="1"/>
-    <col min="28" max="28" width="38.5703125" customWidth="1"/>
-    <col min="29" max="29" width="43.7109375" customWidth="1"/>
-    <col min="30" max="30" width="27.7109375" customWidth="1"/>
-    <col min="31" max="31" width="8.7109375" customWidth="1"/>
-    <col min="32" max="32" width="9" customWidth="1"/>
-    <col min="33" max="33" width="7.28515625" customWidth="1"/>
-    <col min="34" max="34" width="6.42578125" customWidth="1"/>
-    <col min="35" max="35" width="6.7109375" customWidth="1"/>
-    <col min="36" max="36" width="8.28515625" customWidth="1"/>
-    <col min="37" max="37" width="298.42578125" customWidth="1"/>
-    <col min="38" max="38" width="367.42578125" customWidth="1"/>
-    <col min="39" max="39" width="513.140625" customWidth="1"/>
-    <col min="40" max="40" width="20.85546875" customWidth="1"/>
-    <col min="41" max="41" width="78.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="55" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="36" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="152.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="153.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="197.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="79.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
@@ -1779,247 +1720,130 @@
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" t="s">
-        <v>129</v>
-      </c>
-      <c r="I11" t="s">
-        <v>123</v>
-      </c>
-      <c r="J11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" t="s">
-        <v>44</v>
-      </c>
-      <c r="L11" s="1">
-        <v>43252</v>
-      </c>
-      <c r="M11" t="s">
-        <v>130</v>
-      </c>
-      <c r="N11">
-        <v>2017</v>
-      </c>
-      <c r="O11" t="s">
-        <v>41</v>
-      </c>
-      <c r="P11" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>69</v>
-      </c>
-      <c r="T11" t="s">
-        <v>41</v>
-      </c>
-      <c r="W11" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>131</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>132</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>133</v>
-      </c>
-      <c r="AO11" t="s">
-        <v>134</v>
-      </c>
+      <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>136</v>
-      </c>
-      <c r="D12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" t="s">
-        <v>137</v>
-      </c>
-      <c r="J12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" t="s">
-        <v>44</v>
-      </c>
-      <c r="L12" s="1">
-        <v>43115</v>
-      </c>
-      <c r="M12" t="s">
-        <v>138</v>
-      </c>
-      <c r="N12">
-        <v>2017</v>
-      </c>
-      <c r="P12" t="s">
-        <v>45</v>
-      </c>
-      <c r="T12" t="s">
-        <v>41</v>
-      </c>
-      <c r="W12" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL12" t="s">
-        <v>139</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>140</v>
-      </c>
+      <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>142</v>
-      </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" t="s">
-        <v>143</v>
-      </c>
-      <c r="I13" t="s">
-        <v>144</v>
-      </c>
-      <c r="J13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L13" s="1">
-        <v>42943</v>
-      </c>
-      <c r="M13" t="s">
-        <v>145</v>
-      </c>
-      <c r="N13">
-        <v>2017</v>
-      </c>
-      <c r="P13" t="s">
-        <v>45</v>
-      </c>
-      <c r="T13" t="s">
-        <v>41</v>
-      </c>
-      <c r="W13" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>146</v>
-      </c>
-      <c r="AO13" t="s">
-        <v>147</v>
-      </c>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L37" s="1"/>
+    </row>
+    <row r="38" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L38" s="1"/>
+    </row>
+    <row r="39" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L39" s="1"/>
+    </row>
+    <row r="40" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L40" s="1"/>
+    </row>
+    <row r="41" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L42" s="1"/>
+    </row>
+    <row r="43" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L43" s="1"/>
+    </row>
+    <row r="44" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L44" s="1"/>
+    </row>
+    <row r="45" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L45" s="1"/>
+    </row>
+    <row r="46" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L46" s="1"/>
+    </row>
+    <row r="47" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L47" s="1"/>
+    </row>
+    <row r="48" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L48" s="1"/>
+    </row>
+    <row r="49" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L49" s="1"/>
+    </row>
+    <row r="50" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L50" s="1"/>
+    </row>
+    <row r="51" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L51" s="1"/>
+    </row>
+    <row r="52" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L52" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2028,6 +1852,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2036,7 +1866,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BD87EC79D7AB454591EAFECBD90626D9" ma:contentTypeVersion="3" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="0d3d7e2407b21afa2d30d9f4658ecfdd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a15b57ec-90af-49ba-a0a2-d3f0af0f9931" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a24a46ed92df228c743fe265ed7e3ec" ns2:_="">
     <xsd:import namespace="a15b57ec-90af-49ba-a0a2-d3f0af0f9931"/>
@@ -2174,13 +2004,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D55DEAC-2583-419A-AEEA-EE94A1A19F78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F88078F6-43DB-49DB-9553-D1E65F1B4C15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2188,7 +2021,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5D91F3F-1996-4144-8D6F-BAF2247286FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2204,13 +2037,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D55DEAC-2583-419A-AEEA-EE94A1A19F78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactored ConverterService class + updated ToDo's in main
</commit_message>
<xml_diff>
--- a/src/main/java/org/example/util/data/GRI_2017_2020_TEST.xlsx
+++ b/src/main/java/org/example/util/data/GRI_2017_2020_TEST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/35d016b557654f51/Coding/GitHub Desktop Projects/PDF_DOWNLOADER/src/main/java/org/example/util/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="6_{E80B89F1-FD20-43B6-9A20-747F04E0BE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E24A5591-F137-41AE-8F30-CC1E03CD11E9}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="6_{E80B89F1-FD20-43B6-9A20-747F04E0BE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB20D91B-0F70-4052-B689-62C21634B3FA}"/>
   <bookViews>
     <workbookView xWindow="5160" yWindow="1890" windowWidth="41280" windowHeight="17115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AL18" sqref="AL18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,18 +1852,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2005,18 +2005,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D55DEAC-2583-419A-AEEA-EE94A1A19F78}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F88078F6-43DB-49DB-9553-D1E65F1B4C15}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F88078F6-43DB-49DB-9553-D1E65F1B4C15}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D55DEAC-2583-419A-AEEA-EE94A1A19F78}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>